<commit_message>
dodajanje slogov, razpored prepisovanja
</commit_message>
<xml_diff>
--- a/Navodila/Razpored-prepisovanja.xlsx
+++ b/Navodila/Razpored-prepisovanja.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>PREPISOVALEC</t>
   </si>
@@ -81,6 +81,18 @@
   </si>
   <si>
     <t>Klementina Kosi</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>v delu</t>
+  </si>
+  <si>
+    <t>NAPOTNICA</t>
+  </si>
+  <si>
+    <t>DA</t>
   </si>
 </sst>
 </file>
@@ -415,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -426,9 +438,10 @@
     <col min="1" max="1" width="17.77734375" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,8 +451,14 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -449,8 +468,11 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -460,8 +482,11 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -471,8 +496,11 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -483,7 +511,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -493,8 +521,14 @@
       <c r="C6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -504,8 +538,11 @@
       <c r="C7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
dodajanje prepisov in navodil
</commit_message>
<xml_diff>
--- a/Navodila/Razpored-prepisovanja.xlsx
+++ b/Navodila/Razpored-prepisovanja.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>PREPISOVALEC</t>
   </si>
@@ -65,9 +65,6 @@
     <t>f. 97-144</t>
   </si>
   <si>
-    <t>f. 145-191</t>
-  </si>
-  <si>
     <t>s. 18</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
   </si>
   <si>
     <t>s. 261</t>
-  </si>
-  <si>
-    <t>Eva Bonifarti</t>
   </si>
   <si>
     <t>Klementina Kosi</t>
@@ -433,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,10 +452,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -475,10 +469,10 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
         <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -492,10 +486,10 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
         <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -509,10 +503,10 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
         <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -520,13 +514,13 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -537,47 +531,30 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
         <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
združitev delnih prepisov Berkeja, dodajanje novih prepisov
</commit_message>
<xml_diff>
--- a/Navodila/Razpored-prepisovanja.xlsx
+++ b/Navodila/Razpored-prepisovanja.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>PREPISOVALEC</t>
   </si>
@@ -93,6 +93,27 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>UKM Ms 598</t>
+  </si>
+  <si>
+    <t>UKM Ms 139</t>
+  </si>
+  <si>
+    <t>končano</t>
+  </si>
+  <si>
+    <t>s. 20</t>
+  </si>
+  <si>
+    <t>s. 84</t>
+  </si>
+  <si>
+    <t>da</t>
+  </si>
+  <si>
+    <t>f. 145-191</t>
   </si>
 </sst>
 </file>
@@ -118,7 +139,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -128,6 +149,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -144,9 +171,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Navadno" xfId="0" builtinId="0"/>
@@ -427,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -468,8 +496,8 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>18</v>
+      <c r="D2" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="E2" t="s">
         <v>20</v>
@@ -485,8 +513,8 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
-        <v>18</v>
+      <c r="D3" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="E3" t="s">
         <v>20</v>
@@ -517,7 +545,7 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
         <v>22</v>
@@ -533,8 +561,8 @@
       <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
-        <v>18</v>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="E6" t="s">
         <v>20</v>
@@ -555,6 +583,57 @@
       </c>
       <c r="E7" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Berke diplomatični prepis korekture, prepis Volmerja in Sprotuletne vijolice
</commit_message>
<xml_diff>
--- a/Navodila/Razpored-prepisovanja.xlsx
+++ b/Navodila/Razpored-prepisovanja.xlsx
@@ -458,7 +458,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,8 +595,8 @@
       <c r="C8" t="s">
         <v>27</v>
       </c>
-      <c r="D8" t="s">
-        <v>18</v>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="E8" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
dodajanje diplomatičnega prepisa kosijeve in šefove pesmarica
</commit_message>
<xml_diff>
--- a/Navodila/Razpored-prepisovanja.xlsx
+++ b/Navodila/Razpored-prepisovanja.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t>PREPISOVALEC</t>
   </si>
@@ -68,15 +68,9 @@
     <t>s. 18</t>
   </si>
   <si>
-    <t>Klementina Kosi</t>
-  </si>
-  <si>
     <t>STATUS</t>
   </si>
   <si>
-    <t>v delu</t>
-  </si>
-  <si>
     <t>NAPOTNICA</t>
   </si>
   <si>
@@ -108,6 +102,24 @@
   </si>
   <si>
     <t>f. 145-191</t>
+  </si>
+  <si>
+    <t>f. 1-121</t>
+  </si>
+  <si>
+    <t>Markiševska</t>
+  </si>
+  <si>
+    <t>122-244</t>
+  </si>
+  <si>
+    <t>Kosijeva pesmarica</t>
+  </si>
+  <si>
+    <t>Špeka Kovačič</t>
+  </si>
+  <si>
+    <t>Šefova</t>
   </si>
 </sst>
 </file>
@@ -133,7 +145,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,6 +164,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -165,10 +183,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Navadno" xfId="0" builtinId="0"/>
@@ -449,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,10 +493,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -491,10 +510,10 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -508,10 +527,10 @@
         <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -524,11 +543,11 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
         <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -536,13 +555,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -556,15 +572,18 @@
         <v>13</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -572,16 +591,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -589,16 +608,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
         <v>24</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -609,13 +628,49 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="C11" t="s">
         <v>26</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dopolnitev smernic, dodajanje Martjanske II in Sadla
</commit_message>
<xml_diff>
--- a/Navodila/Razpored-prepisovanja.xlsx
+++ b/Navodila/Razpored-prepisovanja.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="44">
   <si>
     <t>PREPISOVALEC</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Martjanska II</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>UKM Ms 598</t>
   </si>
   <si>
@@ -120,6 +117,45 @@
   </si>
   <si>
     <t>Šefova</t>
+  </si>
+  <si>
+    <t>ne</t>
+  </si>
+  <si>
+    <t>Cantiones mortualis</t>
+  </si>
+  <si>
+    <t>celotna</t>
+  </si>
+  <si>
+    <t>Gaberjeva I</t>
+  </si>
+  <si>
+    <t>CELOTNA</t>
+  </si>
+  <si>
+    <t>Gaber-Bokan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Berke </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUK </t>
+  </si>
+  <si>
+    <t>Sara Gomboc</t>
+  </si>
+  <si>
+    <t>Žana Horvat</t>
+  </si>
+  <si>
+    <t>Tina Raj</t>
+  </si>
+  <si>
+    <t>Laura Sobočan</t>
+  </si>
+  <si>
+    <t>Katja Huber</t>
   </si>
 </sst>
 </file>
@@ -468,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,13 +540,13 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
@@ -521,13 +557,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
@@ -538,13 +574,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
@@ -557,8 +593,14 @@
       <c r="B5" t="s">
         <v>17</v>
       </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -572,7 +614,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
         <v>16</v>
@@ -583,7 +625,16 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -591,16 +642,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
         <v>23</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -608,16 +659,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -628,13 +679,13 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -642,35 +693,126 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
         <v>27</v>
       </c>
-      <c r="C12" t="s">
-        <v>28</v>
+      <c r="D12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
         <v>30</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>